<commit_message>
Changes to DAT file and Hiearchy Updation
</commit_message>
<xml_diff>
--- a/Server/Required_files/HDL_BO_Hierarchy_All_Objects_Charlie.xlsx
+++ b/Server/Required_files/HDL_BO_Hierarchy_All_Objects_Charlie.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Charlie\Project_Charlie_v1.10.2\Project_Charlie\Server\Required_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GIT\Project_Charlie_Main\Server\Required_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50AD8D6-BC36-4F87-ACEB-CB994405171D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8040F4-4CC3-4EC2-8D9E-35438D113814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$136</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$137</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="381">
   <si>
     <t>Template Name</t>
   </si>
@@ -1149,6 +1149,39 @@
   </si>
   <si>
     <t>PersonAccrualPlanEnrollment</t>
+  </si>
+  <si>
+    <t>ExternalBankAccountOwner</t>
+  </si>
+  <si>
+    <t>HCM_Time and Labor_Transactional Data_PayrollTimeCard</t>
+  </si>
+  <si>
+    <t>PayrollTimeCard.dat</t>
+  </si>
+  <si>
+    <t>Time and Labor</t>
+  </si>
+  <si>
+    <t>PayrollTimeCard</t>
+  </si>
+  <si>
+    <t>HCM_Time and Labor_Transactional Data_PayrollTimeCard_TimeEntry</t>
+  </si>
+  <si>
+    <t>TimeEntry.dat</t>
+  </si>
+  <si>
+    <t>TimeEntry</t>
+  </si>
+  <si>
+    <t>HCM_Time and Labor_Transactional Data_PayrollTimeCard_TimeEntry_TimeEntryProperty</t>
+  </si>
+  <si>
+    <t>TimeEntryProperty.dat</t>
+  </si>
+  <si>
+    <t>TimeEntryProperty</t>
   </si>
 </sst>
 </file>
@@ -1528,11 +1561,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P136"/>
+  <dimension ref="A1:P140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G134" sqref="G134"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J140" sqref="J140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3731,7 +3764,7 @@
         <v>150</v>
       </c>
       <c r="G75" t="s">
-        <v>177</v>
+        <v>18</v>
       </c>
       <c r="H75" t="s">
         <v>192</v>
@@ -4233,45 +4266,45 @@
       <c r="O91" t="s">
         <v>363</v>
       </c>
-      <c r="P91" t="s">
-        <v>245</v>
-      </c>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B92" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E92" t="s">
         <v>16</v>
       </c>
       <c r="F92" t="s">
-        <v>22</v>
+        <v>150</v>
       </c>
       <c r="G92" t="s">
-        <v>177</v>
+        <v>18</v>
       </c>
       <c r="H92" t="s">
-        <v>248</v>
+        <v>244</v>
+      </c>
+      <c r="I92" t="s">
+        <v>370</v>
       </c>
       <c r="M92" s="1">
         <v>1</v>
       </c>
       <c r="N92" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="O92" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="P92" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B93" t="s">
         <v>247</v>
@@ -4288,16 +4321,22 @@
       <c r="H93" t="s">
         <v>248</v>
       </c>
-      <c r="I93" t="s">
-        <v>251</v>
-      </c>
       <c r="M93" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="N93" t="s">
+        <v>359</v>
+      </c>
+      <c r="O93" t="s">
+        <v>362</v>
+      </c>
+      <c r="P93" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B94" t="s">
         <v>247</v>
@@ -4315,7 +4354,7 @@
         <v>248</v>
       </c>
       <c r="I94" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="M94" s="1">
         <v>0</v>
@@ -4323,7 +4362,7 @@
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B95" t="s">
         <v>247</v>
@@ -4341,7 +4380,7 @@
         <v>248</v>
       </c>
       <c r="I95" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="M95" s="1">
         <v>0</v>
@@ -4349,7 +4388,7 @@
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B96" t="s">
         <v>247</v>
@@ -4367,7 +4406,7 @@
         <v>248</v>
       </c>
       <c r="I96" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="M96" s="1">
         <v>0</v>
@@ -4375,10 +4414,10 @@
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B97" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="E97" t="s">
         <v>16</v>
@@ -4390,56 +4429,50 @@
         <v>177</v>
       </c>
       <c r="H97" t="s">
-        <v>260</v>
+        <v>248</v>
+      </c>
+      <c r="I97" t="s">
+        <v>257</v>
       </c>
       <c r="M97" s="1">
-        <v>1</v>
-      </c>
-      <c r="N97" t="s">
-        <v>359</v>
-      </c>
-      <c r="O97" t="s">
-        <v>363</v>
-      </c>
-      <c r="P97" t="s">
-        <v>261</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B98" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E98" t="s">
         <v>16</v>
       </c>
       <c r="F98" t="s">
-        <v>264</v>
+        <v>22</v>
       </c>
       <c r="G98" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
       <c r="H98" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="M98" s="1">
         <v>1</v>
       </c>
       <c r="N98" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="O98" t="s">
         <v>363</v>
       </c>
       <c r="P98" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B99" t="s">
         <v>263</v>
@@ -4456,16 +4489,22 @@
       <c r="H99" t="s">
         <v>265</v>
       </c>
-      <c r="I99" t="s">
-        <v>268</v>
-      </c>
       <c r="M99" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="N99" t="s">
+        <v>357</v>
+      </c>
+      <c r="O99" t="s">
+        <v>363</v>
+      </c>
+      <c r="P99" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B100" t="s">
         <v>263</v>
@@ -4483,7 +4522,7 @@
         <v>265</v>
       </c>
       <c r="I100" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="M100" s="1">
         <v>0</v>
@@ -4491,7 +4530,7 @@
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B101" t="s">
         <v>263</v>
@@ -4509,7 +4548,7 @@
         <v>265</v>
       </c>
       <c r="I101" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="M101" s="1">
         <v>0</v>
@@ -4517,7 +4556,7 @@
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B102" t="s">
         <v>263</v>
@@ -4535,7 +4574,7 @@
         <v>265</v>
       </c>
       <c r="I102" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="M102" s="1">
         <v>0</v>
@@ -4543,7 +4582,7 @@
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B103" t="s">
         <v>263</v>
@@ -4561,7 +4600,7 @@
         <v>265</v>
       </c>
       <c r="I103" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="M103" s="1">
         <v>0</v>
@@ -4569,39 +4608,33 @@
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B104" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="E104" t="s">
         <v>16</v>
       </c>
       <c r="F104" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="G104" t="s">
         <v>18</v>
       </c>
       <c r="H104" t="s">
-        <v>280</v>
+        <v>265</v>
+      </c>
+      <c r="I104" t="s">
+        <v>276</v>
       </c>
       <c r="M104" s="1">
-        <v>1</v>
-      </c>
-      <c r="N104" t="s">
-        <v>357</v>
-      </c>
-      <c r="O104" t="s">
-        <v>363</v>
-      </c>
-      <c r="P104" t="s">
-        <v>281</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B105" t="s">
         <v>278</v>
@@ -4618,48 +4651,48 @@
       <c r="H105" t="s">
         <v>280</v>
       </c>
-      <c r="I105" t="s">
-        <v>283</v>
-      </c>
       <c r="M105" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="N105" t="s">
+        <v>357</v>
+      </c>
+      <c r="O105" t="s">
+        <v>363</v>
+      </c>
+      <c r="P105" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B106" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="E106" t="s">
         <v>16</v>
       </c>
       <c r="F106" t="s">
-        <v>102</v>
+        <v>279</v>
       </c>
       <c r="G106" t="s">
         <v>18</v>
       </c>
       <c r="H106" t="s">
-        <v>286</v>
+        <v>280</v>
+      </c>
+      <c r="I106" t="s">
+        <v>283</v>
       </c>
       <c r="M106" s="1">
-        <v>1</v>
-      </c>
-      <c r="N106" t="s">
-        <v>357</v>
-      </c>
-      <c r="O106" t="s">
-        <v>363</v>
-      </c>
-      <c r="P106" t="s">
-        <v>287</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B107" t="s">
         <v>285</v>
@@ -4676,16 +4709,22 @@
       <c r="H107" t="s">
         <v>286</v>
       </c>
-      <c r="I107" t="s">
-        <v>289</v>
-      </c>
       <c r="M107" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="N107" t="s">
+        <v>357</v>
+      </c>
+      <c r="O107" t="s">
+        <v>363</v>
+      </c>
+      <c r="P107" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B108" t="s">
         <v>285</v>
@@ -4703,7 +4742,7 @@
         <v>286</v>
       </c>
       <c r="I108" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="M108" s="1">
         <v>0</v>
@@ -4711,7 +4750,7 @@
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B109" t="s">
         <v>285</v>
@@ -4731,16 +4770,13 @@
       <c r="I109" t="s">
         <v>291</v>
       </c>
-      <c r="J109" t="s">
-        <v>293</v>
-      </c>
       <c r="M109" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B110" t="s">
         <v>285</v>
@@ -4761,7 +4797,7 @@
         <v>291</v>
       </c>
       <c r="J110" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="M110" s="1">
         <v>0</v>
@@ -4769,7 +4805,7 @@
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B111" t="s">
         <v>285</v>
@@ -4790,7 +4826,7 @@
         <v>291</v>
       </c>
       <c r="J111" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="M111" s="1">
         <v>0</v>
@@ -4798,7 +4834,7 @@
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B112" t="s">
         <v>285</v>
@@ -4816,7 +4852,10 @@
         <v>286</v>
       </c>
       <c r="I112" t="s">
-        <v>299</v>
+        <v>291</v>
+      </c>
+      <c r="J112" t="s">
+        <v>297</v>
       </c>
       <c r="M112" s="1">
         <v>0</v>
@@ -4824,7 +4863,7 @@
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B113" t="s">
         <v>285</v>
@@ -4842,7 +4881,7 @@
         <v>286</v>
       </c>
       <c r="I113" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="M113" s="1">
         <v>0</v>
@@ -4850,7 +4889,7 @@
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B114" t="s">
         <v>285</v>
@@ -4868,7 +4907,7 @@
         <v>286</v>
       </c>
       <c r="I114" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="M114" s="1">
         <v>0</v>
@@ -4876,7 +4915,7 @@
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B115" t="s">
         <v>285</v>
@@ -4894,7 +4933,7 @@
         <v>286</v>
       </c>
       <c r="I115" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="M115" s="1">
         <v>0</v>
@@ -4902,7 +4941,7 @@
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B116" t="s">
         <v>285</v>
@@ -4920,7 +4959,7 @@
         <v>286</v>
       </c>
       <c r="I116" t="s">
-        <v>128</v>
+        <v>305</v>
       </c>
       <c r="M116" s="1">
         <v>0</v>
@@ -4928,7 +4967,7 @@
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B117" t="s">
         <v>285</v>
@@ -4946,7 +4985,7 @@
         <v>286</v>
       </c>
       <c r="I117" t="s">
-        <v>308</v>
+        <v>128</v>
       </c>
       <c r="M117" s="1">
         <v>0</v>
@@ -4954,7 +4993,7 @@
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B118" t="s">
         <v>285</v>
@@ -4972,7 +5011,7 @@
         <v>286</v>
       </c>
       <c r="I118" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="M118" s="1">
         <v>0</v>
@@ -4980,7 +5019,7 @@
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B119" t="s">
         <v>285</v>
@@ -4998,21 +5037,15 @@
         <v>286</v>
       </c>
       <c r="I119" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="M119" s="1">
-        <v>1</v>
-      </c>
-      <c r="N119" t="s">
-        <v>357</v>
-      </c>
-      <c r="O119" t="s">
-        <v>363</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B120" t="s">
         <v>285</v>
@@ -5030,15 +5063,21 @@
         <v>286</v>
       </c>
       <c r="I120" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="M120" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="N120" t="s">
+        <v>357</v>
+      </c>
+      <c r="O120" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B121" t="s">
         <v>285</v>
@@ -5056,7 +5095,7 @@
         <v>286</v>
       </c>
       <c r="I121" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="M121" s="1">
         <v>0</v>
@@ -5064,39 +5103,33 @@
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B122" t="s">
-        <v>318</v>
+        <v>285</v>
       </c>
       <c r="E122" t="s">
         <v>16</v>
       </c>
       <c r="F122" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="G122" t="s">
-        <v>177</v>
+        <v>18</v>
       </c>
       <c r="H122" t="s">
-        <v>319</v>
+        <v>286</v>
+      </c>
+      <c r="I122" t="s">
+        <v>316</v>
       </c>
       <c r="M122" s="1">
-        <v>1</v>
-      </c>
-      <c r="N122" t="s">
-        <v>357</v>
-      </c>
-      <c r="O122" t="s">
-        <v>362</v>
-      </c>
-      <c r="P122" t="s">
-        <v>320</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B123" t="s">
         <v>318</v>
@@ -5113,16 +5146,22 @@
       <c r="H123" t="s">
         <v>319</v>
       </c>
-      <c r="I123" t="s">
-        <v>322</v>
-      </c>
       <c r="M123" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="N123" t="s">
+        <v>357</v>
+      </c>
+      <c r="O123" t="s">
+        <v>362</v>
+      </c>
+      <c r="P123" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B124" t="s">
         <v>318</v>
@@ -5140,7 +5179,7 @@
         <v>319</v>
       </c>
       <c r="I124" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="M124" s="1">
         <v>0</v>
@@ -5148,7 +5187,7 @@
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B125" t="s">
         <v>318</v>
@@ -5166,7 +5205,7 @@
         <v>319</v>
       </c>
       <c r="I125" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="M125" s="1">
         <v>0</v>
@@ -5174,39 +5213,33 @@
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B126" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="E126" t="s">
         <v>16</v>
       </c>
       <c r="F126" t="s">
-        <v>279</v>
+        <v>22</v>
       </c>
       <c r="G126" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
       <c r="H126" t="s">
-        <v>329</v>
+        <v>319</v>
+      </c>
+      <c r="I126" t="s">
+        <v>326</v>
       </c>
       <c r="M126" s="1">
-        <v>1</v>
-      </c>
-      <c r="N126" t="s">
-        <v>357</v>
-      </c>
-      <c r="O126" t="s">
-        <v>363</v>
-      </c>
-      <c r="P126" t="s">
-        <v>330</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B127" t="s">
         <v>328</v>
@@ -5223,16 +5256,22 @@
       <c r="H127" t="s">
         <v>329</v>
       </c>
-      <c r="I127" t="s">
-        <v>332</v>
-      </c>
       <c r="M127" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="N127" t="s">
+        <v>357</v>
+      </c>
+      <c r="O127" t="s">
+        <v>363</v>
+      </c>
+      <c r="P127" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B128" t="s">
         <v>328</v>
@@ -5250,7 +5289,7 @@
         <v>329</v>
       </c>
       <c r="I128" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="M128" s="1">
         <v>0</v>
@@ -5258,7 +5297,7 @@
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B129" t="s">
         <v>328</v>
@@ -5276,7 +5315,7 @@
         <v>329</v>
       </c>
       <c r="I129" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M129" s="1">
         <v>0</v>
@@ -5284,10 +5323,10 @@
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>367</v>
+        <v>335</v>
       </c>
       <c r="B130" t="s">
-        <v>368</v>
+        <v>328</v>
       </c>
       <c r="E130" t="s">
         <v>16</v>
@@ -5299,15 +5338,21 @@
         <v>18</v>
       </c>
       <c r="H130" t="s">
-        <v>369</v>
+        <v>329</v>
+      </c>
+      <c r="I130" t="s">
+        <v>336</v>
+      </c>
+      <c r="M130" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="B131" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="E131" t="s">
         <v>16</v>
@@ -5316,47 +5361,35 @@
         <v>279</v>
       </c>
       <c r="G131" t="s">
-        <v>177</v>
+        <v>18</v>
       </c>
       <c r="H131" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>337</v>
+        <v>364</v>
       </c>
       <c r="B132" t="s">
-        <v>338</v>
+        <v>366</v>
       </c>
       <c r="E132" t="s">
         <v>16</v>
       </c>
       <c r="F132" t="s">
-        <v>22</v>
+        <v>279</v>
       </c>
       <c r="G132" t="s">
         <v>177</v>
       </c>
       <c r="H132" t="s">
-        <v>339</v>
-      </c>
-      <c r="M132" s="1">
-        <v>1</v>
-      </c>
-      <c r="N132" t="s">
-        <v>361</v>
-      </c>
-      <c r="O132" t="s">
-        <v>362</v>
-      </c>
-      <c r="P132" t="s">
-        <v>340</v>
+        <v>365</v>
       </c>
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B133" t="s">
         <v>338</v>
@@ -5373,16 +5406,22 @@
       <c r="H133" t="s">
         <v>339</v>
       </c>
-      <c r="I133" t="s">
-        <v>342</v>
-      </c>
       <c r="M133" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="N133" t="s">
+        <v>361</v>
+      </c>
+      <c r="O133" t="s">
+        <v>362</v>
+      </c>
+      <c r="P133" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B134" t="s">
         <v>338</v>
@@ -5400,7 +5439,7 @@
         <v>339</v>
       </c>
       <c r="I134" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="M134" s="1">
         <v>0</v>
@@ -5408,54 +5447,48 @@
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B135" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="E135" t="s">
         <v>16</v>
       </c>
       <c r="F135" t="s">
-        <v>279</v>
+        <v>22</v>
       </c>
       <c r="G135" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
       <c r="H135" t="s">
-        <v>347</v>
+        <v>339</v>
+      </c>
+      <c r="I135" t="s">
+        <v>344</v>
       </c>
       <c r="M135" s="1">
-        <v>1</v>
-      </c>
-      <c r="N135" t="s">
-        <v>357</v>
-      </c>
-      <c r="O135" t="s">
-        <v>363</v>
-      </c>
-      <c r="P135" t="s">
-        <v>348</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="B136" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="E136" t="s">
         <v>16</v>
       </c>
       <c r="F136" t="s">
-        <v>150</v>
+        <v>279</v>
       </c>
       <c r="G136" t="s">
         <v>18</v>
       </c>
       <c r="H136" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="M136" s="1">
         <v>1</v>
@@ -5467,14 +5500,116 @@
         <v>363</v>
       </c>
       <c r="P136" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="137" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>349</v>
+      </c>
+      <c r="B137" t="s">
+        <v>350</v>
+      </c>
+      <c r="E137" t="s">
+        <v>16</v>
+      </c>
+      <c r="F137" t="s">
+        <v>150</v>
+      </c>
+      <c r="G137" t="s">
+        <v>18</v>
+      </c>
+      <c r="H137" t="s">
+        <v>351</v>
+      </c>
+      <c r="M137" s="1">
+        <v>1</v>
+      </c>
+      <c r="N137" t="s">
+        <v>357</v>
+      </c>
+      <c r="O137" t="s">
+        <v>363</v>
+      </c>
+      <c r="P137" t="s">
         <v>352</v>
       </c>
     </row>
+    <row r="138" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>371</v>
+      </c>
+      <c r="B138" t="s">
+        <v>372</v>
+      </c>
+      <c r="E138" t="s">
+        <v>16</v>
+      </c>
+      <c r="F138" t="s">
+        <v>373</v>
+      </c>
+      <c r="G138" t="s">
+        <v>18</v>
+      </c>
+      <c r="H138" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="139" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>375</v>
+      </c>
+      <c r="B139" t="s">
+        <v>376</v>
+      </c>
+      <c r="E139" t="s">
+        <v>16</v>
+      </c>
+      <c r="F139" t="s">
+        <v>373</v>
+      </c>
+      <c r="G139" t="s">
+        <v>18</v>
+      </c>
+      <c r="H139" t="s">
+        <v>374</v>
+      </c>
+      <c r="I139" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="140" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>378</v>
+      </c>
+      <c r="B140" t="s">
+        <v>379</v>
+      </c>
+      <c r="E140" t="s">
+        <v>16</v>
+      </c>
+      <c r="F140" t="s">
+        <v>373</v>
+      </c>
+      <c r="G140" t="s">
+        <v>18</v>
+      </c>
+      <c r="H140" t="s">
+        <v>374</v>
+      </c>
+      <c r="I140" t="s">
+        <v>377</v>
+      </c>
+      <c r="J140" t="s">
+        <v>380</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:P137" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:M1 A3:M36 A2:L2 A108:L118 A38 C38:L38 A39:L39 A40:L59 A60:L60 A61:L61 A62:L63 A64 C64:L64 A65:L65 A66:L67 A68:L68 A69:L69 A70:L70 A71:L71 A72:L72 A73:L73 A74:L74 A75 C75:L75 A76:L76 A77:L77 A78:L81 A82:G82 I82:L82 A83:L83 A84:L84 A85:L85 A86:G86 I86:L86 A87:L87 A88:L88 A89:L89 A90:L90 A91:L91 A92:L92 A93:L93 A94:L96 A97:L97 A98:L98 A99:L99 A100:L103 A104:G104 I104:L104 A105:L105 A106:L106 A136:L136 A119:L119 A107:L107 A120:L120 A121:L121 A122:L122 A123:L123 A124:L125 A126:G126 I126:L126 A127:L127 A128:L129 A132:L132 A133:L133 A134:L134 A135:G135 I135:L135 A37:L37" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:M1 A3:M36 A2:L2 A109:L119 A38 C38:L38 A39:L39 A40:L59 A60:L60 A61:L61 A62:L63 A64 C64:L64 A65:L65 A66:L67 A68:L68 A69:L69 A70:L70 A71:L71 A72:L72 A73:L73 A74:L74 A75 C75:F75 A76:L76 A77:L77 A78:L81 A82:G82 I82:L82 A83:L83 A84:L84 A85:L85 A86:G86 I86:L86 A87:L87 A88:L88 A89:L89 A90:L90 A92:H92 A93:L93 A94:L94 A95:L97 A98:L98 A99:L99 A100:L100 A101:L104 A105:G105 I105:L105 A106:L106 A107:L107 A137:L137 A120:L120 A108:L108 A121:L121 A122:L122 A123:L123 A124:L124 A125:L126 A127:G127 I127:L127 A128:L128 A129:L130 A133:L133 A134:L134 A135:L135 A136:G136 I136:L136 A37:L37 H75:L75 J92:L92" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -5486,15 +5621,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004EAF5FBB9A618A49A458E02053155296" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7446135c09aed1d59234afa5e6d033ad">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="eda7b593-5b33-4455-9f72-a492af41ea7a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="45ba4306679ce686ee2f31d42500edb0" ns2:_="">
     <xsd:import namespace="eda7b593-5b33-4455-9f72-a492af41ea7a"/>
@@ -5656,6 +5782,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3604BF4-0FFF-4404-B039-B7C228E8F270}">
   <ds:schemaRefs>
@@ -5673,14 +5808,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DD9110C-7E4A-451C-B6FE-5459C4D27920}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCC09508-E555-4D09-A733-337E37140E03}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5696,4 +5823,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DD9110C-7E4A-451C-B6FE-5459C4D27920}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>